<commit_message>
Update Matrice de repartition des tâches.xlsx
</commit_message>
<xml_diff>
--- a/Livrables/Matrice de repartition des tâches.xlsx
+++ b/Livrables/Matrice de repartition des tâches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/GitHub/Covid-19_Progression_Modeler/Livrables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1D7F419-1F7D-DC41-93E0-1AC64428BD90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC7F51-6261-4C4F-B837-04697B20C2FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
   <si>
     <t>Qualité des livrables</t>
   </si>
@@ -46,13 +46,7 @@
     <t>INTITULÉ DU PROJET</t>
   </si>
   <si>
-    <t>CHEF DE PROJETS</t>
-  </si>
-  <si>
     <t>NOM DE L’ENTREPRISE</t>
-  </si>
-  <si>
-    <t>DATE</t>
   </si>
   <si>
     <t>TÂCHE</t>
@@ -251,13 +245,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -393,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -605,17 +598,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top/>
@@ -694,21 +676,6 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </left>
-      <right style="hair">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34995574816125979"/>
-      </top>
-      <bottom style="double">
         <color theme="0" tint="-0.34995574816125979"/>
       </bottom>
       <diagonal/>
@@ -934,7 +901,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -957,36 +924,30 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -994,31 +955,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1027,25 +988,19 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1054,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1066,34 +1021,34 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1347,11 +1302,11 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:G40"/>
+  <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,601 +1319,581 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="2:7" s="1" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+      <c r="B1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="2:7" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>54</v>
+      <c r="C2" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="2:7" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="2:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>55</v>
-      </c>
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+    <row r="5" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="2:7" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="28" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="29" t="s">
+      <c r="F7" s="31"/>
+      <c r="G7" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="30" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="49" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
+      <c r="F9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="53" t="s">
+      <c r="C12" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="E12" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="53" t="s">
+      <c r="D13" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="E15" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="16" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>66</v>
-      </c>
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="53" t="s">
+    </row>
+    <row r="18" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="E18" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8">
-        <v>2</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="53" t="s">
+      <c r="D19" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>67</v>
+      <c r="E19" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="53" t="s">
+      <c r="D20" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>68</v>
+      <c r="E20" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>68</v>
-      </c>
+      <c r="B21" s="8">
+        <v>3</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="53" t="s">
+      <c r="D23" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="E23" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="8">
-        <v>3</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="41" t="s">
+      <c r="B24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="53" t="s">
+      <c r="D24" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="E24" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="25" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="53" t="s">
+      <c r="D25" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="E25" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="26" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="53" t="s">
+      <c r="C26" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="E26" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="27" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="53" t="s">
+      <c r="C27" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="E27" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="17" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="28" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="41" t="s">
+      <c r="B28" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="53" t="s">
+      <c r="D28" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="E28" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="20" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="29" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="41" t="s">
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="C32" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="53" t="s">
+      <c r="D32" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="E32" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="51" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="53" t="s">
+    </row>
+    <row r="33" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="51" t="s">
+      <c r="E33" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="8">
-        <v>4</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="8">
-        <v>4.3</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="C40" s="2"/>
+    </row>
+    <row r="38" spans="2:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="C38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
@@ -1979,14 +1914,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" style="22" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="22"/>
+    <col min="1" max="1" width="3.33203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:2" ht="161" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>